<commit_message>
•	ID 29, 37, 64, 66, 67, 68, 69, 70, 73,  la procedura adottata per la risoluzione dell’errore e le modalità di invio successivo del documento al FSE, considerato che si sta descrivendo la gestione dell’errore nel processo di validazione.
•	ID 63, 65, il criterio e la modalità con cui viene gestita da un operatore di backoffice la correzione del confidentialityCode, trattandosi di un attributo impostato dall’utente (medico);  inoltre, chiarire le modalità di invio del documento al FSE a seguito della risoluzione dell’errore
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/asl2savonese/onesys/2.6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/asl2savonese/onesys/2.6.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACCREDITAMENTO_FSE_ONESYS\GATEWAY\A1#111ELCO0000000\asl2savonese\onesys\2.6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F300684-A7AA-4D6B-B808-3B578BF31BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C231B1-9D15-4CE3-AB5C-BA8929DB4970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="886">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4470,9 +4470,6 @@
     <t>2.16.840.1.113883.2.9.2.70102.5d1e9ebb3bdc671786398ac1e5eedda1cb5efd65305d8ed602199337510cdd3e.9e9f62d536^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Occorre Rifirmare la lettera dopo aver corretto l'errore</t>
-  </si>
-  <si>
     <t>2023-05-24T09:19:28.644Z</t>
   </si>
   <si>
@@ -4611,7 +4608,14 @@
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 00558]</t>
   </si>
   <si>
-    <t>Il sistema prosegue nella firma. Nel caso in cui la regione abbia un metodo di rivalidazione sui repository/nodi centrali viene demandato a questo la validazione. In alternativa occore rifirmare il referto</t>
+    <t>Tramite apposito cruscotto sul software di BI potrà essere preso in carico l'errore, corretto il campo da interfaccia e reinviato il referto</t>
+  </si>
+  <si>
+    <t>Tramite apposito cruscotto sul software di BI potrà essere preso in carico l'errore, corretto il campo da interfaccia e reinviato il referto  Occorre nuova Firma dopo correzzione in quanto il dato è contenuto all'interno del CDA2</t>
+  </si>
+  <si>
+    <t>Il sistema attende un numero di millisecondi configurabile (default 5000) Dopo tale tempo viene mostrato un messaggio di errore al medico ed è configurabile il fatto di interrompere il processo o permettere al medico di firmare il referto. Il pdf risultante avrà comunque al suo interno il cda2
+In automatico prima di inviare a fse o al repository viene tentata nuova validazione</t>
   </si>
 </sst>
 </file>
@@ -7528,10 +7532,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="D194" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="I252" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J246" sqref="J246"/>
+      <selection pane="bottomRight" activeCell="Q228" sqref="Q228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14693,13 +14697,13 @@
         <v>45070</v>
       </c>
       <c r="G212" s="24" t="s">
+        <v>837</v>
+      </c>
+      <c r="H212" s="24" t="s">
         <v>838</v>
       </c>
-      <c r="H212" s="24" t="s">
+      <c r="I212" s="24" t="s">
         <v>839</v>
-      </c>
-      <c r="I212" s="24" t="s">
-        <v>840</v>
       </c>
       <c r="J212" s="25" t="s">
         <v>489</v>
@@ -14712,13 +14716,13 @@
         <v>489</v>
       </c>
       <c r="N212" s="25" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="O212" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P212" s="25" t="s">
-        <v>837</v>
+        <v>883</v>
       </c>
       <c r="Q212" s="25"/>
       <c r="R212" s="26"/>
@@ -14985,13 +14989,13 @@
         <v>45070</v>
       </c>
       <c r="G220" s="24" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="H220" s="24" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I220" s="24" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="J220" s="25" t="s">
         <v>489</v>
@@ -15004,13 +15008,13 @@
         <v>489</v>
       </c>
       <c r="N220" s="25" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="O220" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P220" s="25" t="s">
-        <v>837</v>
+        <v>883</v>
       </c>
       <c r="Q220" s="25"/>
       <c r="R220" s="26"/>
@@ -15259,7 +15263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="120.75" thickBot="1">
+    <row r="228" spans="1:20" ht="240.75" thickBot="1">
       <c r="A228" s="20">
         <v>45</v>
       </c>
@@ -15288,11 +15292,11 @@
       <c r="L228" s="25"/>
       <c r="M228" s="25"/>
       <c r="N228" s="25" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="O228" s="25"/>
       <c r="P228" s="25" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="Q228" s="25"/>
       <c r="R228" s="26" t="s">
@@ -15893,7 +15897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="120.75" thickBot="1">
+    <row r="246" spans="1:20" ht="135.75" thickBot="1">
       <c r="A246" s="20">
         <v>63</v>
       </c>
@@ -15913,13 +15917,13 @@
         <v>45070</v>
       </c>
       <c r="G246" s="24" t="s">
+        <v>845</v>
+      </c>
+      <c r="H246" s="24" t="s">
+        <v>847</v>
+      </c>
+      <c r="I246" s="24" t="s">
         <v>846</v>
-      </c>
-      <c r="H246" s="24" t="s">
-        <v>848</v>
-      </c>
-      <c r="I246" s="24" t="s">
-        <v>847</v>
       </c>
       <c r="J246" s="25" t="s">
         <v>489</v>
@@ -15932,13 +15936,13 @@
         <v>489</v>
       </c>
       <c r="N246" s="25" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="O246" s="25" t="s">
         <v>489</v>
       </c>
-      <c r="P246" s="25" t="s">
-        <v>837</v>
+      <c r="P246" s="35" t="s">
+        <v>884</v>
       </c>
       <c r="Q246" s="25"/>
       <c r="R246" s="26"/>
@@ -15947,7 +15951,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="120.75" thickBot="1">
+    <row r="247" spans="1:20" ht="135.75" thickBot="1">
       <c r="A247" s="20">
         <v>64</v>
       </c>
@@ -15967,13 +15971,13 @@
         <v>45070</v>
       </c>
       <c r="G247" s="34" t="s">
+        <v>849</v>
+      </c>
+      <c r="H247" s="34" t="s">
         <v>850</v>
       </c>
-      <c r="H247" s="34" t="s">
+      <c r="I247" s="34" t="s">
         <v>851</v>
-      </c>
-      <c r="I247" s="34" t="s">
-        <v>852</v>
       </c>
       <c r="J247" s="35" t="s">
         <v>489</v>
@@ -15986,13 +15990,13 @@
         <v>489</v>
       </c>
       <c r="N247" s="35" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="O247" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P247" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q247" s="25"/>
       <c r="R247" s="26"/>
@@ -16001,7 +16005,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="120.75" thickBot="1">
+    <row r="248" spans="1:20" ht="135.75" thickBot="1">
       <c r="A248" s="20">
         <v>65</v>
       </c>
@@ -16021,13 +16025,13 @@
         <v>45070</v>
       </c>
       <c r="G248" s="34" t="s">
+        <v>853</v>
+      </c>
+      <c r="H248" s="34" t="s">
         <v>854</v>
       </c>
-      <c r="H248" s="34" t="s">
+      <c r="I248" s="34" t="s">
         <v>855</v>
-      </c>
-      <c r="I248" s="34" t="s">
-        <v>856</v>
       </c>
       <c r="J248" s="35" t="s">
         <v>489</v>
@@ -16040,13 +16044,13 @@
         <v>489</v>
       </c>
       <c r="N248" s="35" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="O248" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P248" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q248" s="25"/>
       <c r="R248" s="26"/>
@@ -16055,7 +16059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="120.75" thickBot="1">
+    <row r="249" spans="1:20" ht="135.75" thickBot="1">
       <c r="A249" s="20">
         <v>66</v>
       </c>
@@ -16075,13 +16079,13 @@
         <v>45070</v>
       </c>
       <c r="G249" s="34" t="s">
+        <v>857</v>
+      </c>
+      <c r="H249" s="34" t="s">
         <v>858</v>
       </c>
-      <c r="H249" s="34" t="s">
+      <c r="I249" s="34" t="s">
         <v>859</v>
-      </c>
-      <c r="I249" s="34" t="s">
-        <v>860</v>
       </c>
       <c r="J249" s="35" t="s">
         <v>489</v>
@@ -16094,13 +16098,13 @@
         <v>489</v>
       </c>
       <c r="N249" s="35" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O249" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P249" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q249" s="25"/>
       <c r="R249" s="26"/>
@@ -16109,7 +16113,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="120.75" thickBot="1">
+    <row r="250" spans="1:20" ht="135.75" thickBot="1">
       <c r="A250" s="20">
         <v>67</v>
       </c>
@@ -16129,13 +16133,13 @@
         <v>45070</v>
       </c>
       <c r="G250" s="34" t="s">
+        <v>861</v>
+      </c>
+      <c r="H250" s="34" t="s">
         <v>862</v>
       </c>
-      <c r="H250" s="34" t="s">
+      <c r="I250" s="34" t="s">
         <v>863</v>
-      </c>
-      <c r="I250" s="34" t="s">
-        <v>864</v>
       </c>
       <c r="J250" s="35" t="s">
         <v>489</v>
@@ -16148,13 +16152,13 @@
         <v>489</v>
       </c>
       <c r="N250" s="35" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="O250" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P250" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q250" s="25"/>
       <c r="R250" s="26"/>
@@ -16163,7 +16167,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="120.75" thickBot="1">
+    <row r="251" spans="1:20" ht="135.75" thickBot="1">
       <c r="A251" s="20">
         <v>68</v>
       </c>
@@ -16183,13 +16187,13 @@
         <v>45070</v>
       </c>
       <c r="G251" s="34" t="s">
+        <v>865</v>
+      </c>
+      <c r="H251" s="34" t="s">
         <v>866</v>
       </c>
-      <c r="H251" s="34" t="s">
+      <c r="I251" s="34" t="s">
         <v>867</v>
-      </c>
-      <c r="I251" s="34" t="s">
-        <v>868</v>
       </c>
       <c r="J251" s="35" t="s">
         <v>489</v>
@@ -16202,13 +16206,13 @@
         <v>489</v>
       </c>
       <c r="N251" s="35" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="O251" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P251" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q251" s="25"/>
       <c r="R251" s="26"/>
@@ -16237,13 +16241,13 @@
         <v>45070</v>
       </c>
       <c r="G252" s="34" t="s">
+        <v>869</v>
+      </c>
+      <c r="H252" s="34" t="s">
         <v>870</v>
       </c>
-      <c r="H252" s="34" t="s">
+      <c r="I252" s="34" t="s">
         <v>871</v>
-      </c>
-      <c r="I252" s="34" t="s">
-        <v>872</v>
       </c>
       <c r="J252" s="35" t="s">
         <v>489</v>
@@ -16256,13 +16260,13 @@
         <v>489</v>
       </c>
       <c r="N252" s="35" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="O252" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P252" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q252" s="25"/>
       <c r="R252" s="26"/>
@@ -16271,7 +16275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="120.75" thickBot="1">
+    <row r="253" spans="1:20" ht="135.75" thickBot="1">
       <c r="A253" s="20">
         <v>70</v>
       </c>
@@ -16291,13 +16295,13 @@
         <v>45070</v>
       </c>
       <c r="G253" s="34" t="s">
+        <v>873</v>
+      </c>
+      <c r="H253" s="34" t="s">
         <v>874</v>
       </c>
-      <c r="H253" s="34" t="s">
+      <c r="I253" s="34" t="s">
         <v>875</v>
-      </c>
-      <c r="I253" s="34" t="s">
-        <v>876</v>
       </c>
       <c r="J253" s="35" t="s">
         <v>489</v>
@@ -16310,13 +16314,13 @@
         <v>489</v>
       </c>
       <c r="N253" s="35" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="O253" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P253" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q253" s="25"/>
       <c r="R253" s="26"/>
@@ -16349,7 +16353,7 @@
         <v>829</v>
       </c>
       <c r="K254" s="35" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L254" s="25"/>
       <c r="M254" s="25"/>
@@ -16387,7 +16391,7 @@
         <v>829</v>
       </c>
       <c r="K255" s="35" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="L255" s="25"/>
       <c r="M255" s="25"/>
@@ -16401,7 +16405,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="120.75" thickBot="1">
+    <row r="256" spans="1:20" ht="135.75" thickBot="1">
       <c r="A256" s="20">
         <v>73</v>
       </c>
@@ -16421,13 +16425,13 @@
         <v>45070</v>
       </c>
       <c r="G256" s="34" t="s">
+        <v>879</v>
+      </c>
+      <c r="H256" s="34" t="s">
         <v>880</v>
       </c>
-      <c r="H256" s="34" t="s">
+      <c r="I256" s="34" t="s">
         <v>881</v>
-      </c>
-      <c r="I256" s="34" t="s">
-        <v>882</v>
       </c>
       <c r="J256" s="35" t="s">
         <v>489</v>
@@ -16440,13 +16444,13 @@
         <v>489</v>
       </c>
       <c r="N256" s="35" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="O256" s="25" t="s">
         <v>489</v>
       </c>
       <c r="P256" s="35" t="s">
-        <v>837</v>
+        <v>884</v>
       </c>
       <c r="Q256" s="25"/>
       <c r="R256" s="26"/>
@@ -16479,7 +16483,7 @@
         <v>829</v>
       </c>
       <c r="K257" s="35" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="L257" s="25"/>
       <c r="M257" s="25"/>

</xml_diff>